<commit_message>
feat: add info docs
</commit_message>
<xml_diff>
--- a/IA/app/data/Resultado_Churn.xlsx
+++ b/IA/app/data/Resultado_Churn.xlsx
@@ -1601,7 +1601,7 @@
         </is>
       </c>
       <c r="B90" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C90" t="n">
         <v>0</v>
@@ -1952,7 +1952,7 @@
         </is>
       </c>
       <c r="B117" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C117" t="n">
         <v>1</v>
@@ -1965,7 +1965,7 @@
         </is>
       </c>
       <c r="B118" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C118" t="n">
         <v>0</v>
@@ -2134,7 +2134,7 @@
         </is>
       </c>
       <c r="B131" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C131" t="n">
         <v>0</v>
@@ -2238,7 +2238,7 @@
         </is>
       </c>
       <c r="B139" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C139" t="n">
         <v>0</v>
@@ -2602,7 +2602,7 @@
         </is>
       </c>
       <c r="B167" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C167" t="n">
         <v>0</v>
@@ -3148,7 +3148,7 @@
         </is>
       </c>
       <c r="B209" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C209" t="n">
         <v>0</v>
@@ -3343,7 +3343,7 @@
         </is>
       </c>
       <c r="B224" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C224" t="n">
         <v>0</v>
@@ -4097,7 +4097,7 @@
         </is>
       </c>
       <c r="B282" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C282" t="n">
         <v>0</v>
@@ -5020,7 +5020,7 @@
         </is>
       </c>
       <c r="B353" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C353" t="n">
         <v>0</v>
@@ -5111,7 +5111,7 @@
         </is>
       </c>
       <c r="B360" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C360" t="n">
         <v>0</v>
@@ -6554,7 +6554,7 @@
         </is>
       </c>
       <c r="B471" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C471" t="n">
         <v>0</v>
@@ -8816,7 +8816,7 @@
         </is>
       </c>
       <c r="B645" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C645" t="n">
         <v>0</v>
@@ -9674,7 +9674,7 @@
         </is>
       </c>
       <c r="B711" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C711" t="n">
         <v>0</v>
@@ -10038,7 +10038,7 @@
         </is>
       </c>
       <c r="B739" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C739" t="n">
         <v>0</v>
@@ -10103,7 +10103,7 @@
         </is>
       </c>
       <c r="B744" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C744" t="n">
         <v>0</v>
@@ -10974,7 +10974,7 @@
         </is>
       </c>
       <c r="B811" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C811" t="n">
         <v>0</v>
@@ -11156,7 +11156,7 @@
         </is>
       </c>
       <c r="B825" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C825" t="n">
         <v>0</v>
@@ -11975,7 +11975,7 @@
         </is>
       </c>
       <c r="B888" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C888" t="n">
         <v>0</v>
@@ -14107,7 +14107,7 @@
         </is>
       </c>
       <c r="B1052" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C1052" t="n">
         <v>0</v>
@@ -15186,7 +15186,7 @@
         </is>
       </c>
       <c r="B1135" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C1135" t="n">
         <v>0</v>
@@ -15433,7 +15433,7 @@
         </is>
       </c>
       <c r="B1154" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C1154" t="n">
         <v>0</v>
@@ -15654,7 +15654,7 @@
         </is>
       </c>
       <c r="B1171" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C1171" t="n">
         <v>0</v>
@@ -16356,7 +16356,7 @@
         </is>
       </c>
       <c r="B1225" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C1225" t="n">
         <v>0</v>
@@ -18436,7 +18436,7 @@
         </is>
       </c>
       <c r="B1385" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C1385" t="n">
         <v>0</v>
@@ -19060,7 +19060,7 @@
         </is>
       </c>
       <c r="B1433" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C1433" t="n">
         <v>0</v>
@@ -19645,7 +19645,7 @@
         </is>
       </c>
       <c r="B1478" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C1478" t="n">
         <v>0</v>
@@ -21322,7 +21322,7 @@
         </is>
       </c>
       <c r="B1607" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C1607" t="n">
         <v>0</v>
@@ -21803,7 +21803,7 @@
         </is>
       </c>
       <c r="B1644" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C1644" t="n">
         <v>0</v>
@@ -22037,7 +22037,7 @@
         </is>
       </c>
       <c r="B1662" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C1662" t="n">
         <v>0</v>
@@ -22375,7 +22375,7 @@
         </is>
       </c>
       <c r="B1688" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C1688" t="n">
         <v>0</v>
@@ -23181,7 +23181,7 @@
         </is>
       </c>
       <c r="B1750" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C1750" t="n">
         <v>0</v>
@@ -23389,7 +23389,7 @@
         </is>
       </c>
       <c r="B1766" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C1766" t="n">
         <v>0</v>
@@ -24299,7 +24299,7 @@
         </is>
       </c>
       <c r="B1836" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C1836" t="n">
         <v>0</v>
@@ -24728,7 +24728,7 @@
         </is>
       </c>
       <c r="B1869" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C1869" t="n">
         <v>0</v>
@@ -24910,7 +24910,7 @@
         </is>
       </c>
       <c r="B1883" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C1883" t="n">
         <v>0</v>
@@ -25989,7 +25989,7 @@
         </is>
       </c>
       <c r="B1966" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C1966" t="n">
         <v>0</v>
@@ -28381,7 +28381,7 @@
         </is>
       </c>
       <c r="B2150" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2150" t="n">
         <v>0</v>
@@ -29616,7 +29616,7 @@
         </is>
       </c>
       <c r="B2245" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2245" t="n">
         <v>0</v>
@@ -29785,7 +29785,7 @@
         </is>
       </c>
       <c r="B2258" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2258" t="n">
         <v>0</v>
@@ -30409,7 +30409,7 @@
         </is>
       </c>
       <c r="B2306" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2306" t="n">
         <v>0</v>
@@ -30851,7 +30851,7 @@
         </is>
       </c>
       <c r="B2340" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2340" t="n">
         <v>0</v>
@@ -31995,7 +31995,7 @@
         </is>
       </c>
       <c r="B2428" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2428" t="n">
         <v>0</v>
@@ -32398,7 +32398,7 @@
         </is>
       </c>
       <c r="B2459" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2459" t="n">
         <v>0</v>
@@ -33217,7 +33217,7 @@
         </is>
       </c>
       <c r="B2522" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2522" t="n">
         <v>0</v>
@@ -34712,7 +34712,7 @@
         </is>
       </c>
       <c r="B2637" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2637" t="n">
         <v>0</v>
@@ -35050,7 +35050,7 @@
         </is>
       </c>
       <c r="B2663" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2663" t="n">
         <v>0</v>
@@ -35375,7 +35375,7 @@
         </is>
       </c>
       <c r="B2688" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2688" t="n">
         <v>0</v>
@@ -36259,7 +36259,7 @@
         </is>
       </c>
       <c r="B2756" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2756" t="n">
         <v>0</v>
@@ -36415,7 +36415,7 @@
         </is>
       </c>
       <c r="B2768" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2768" t="n">
         <v>0</v>
@@ -38014,7 +38014,7 @@
         </is>
       </c>
       <c r="B2891" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2891" t="n">
         <v>0</v>
@@ -38807,7 +38807,7 @@
         </is>
       </c>
       <c r="B2952" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2952" t="n">
         <v>0</v>
@@ -41420,7 +41420,7 @@
         </is>
       </c>
       <c r="B3153" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C3153" t="n">
         <v>0</v>
@@ -42603,7 +42603,7 @@
         </is>
       </c>
       <c r="B3244" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C3244" t="n">
         <v>0</v>
@@ -42876,7 +42876,7 @@
         </is>
       </c>
       <c r="B3265" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C3265" t="n">
         <v>0</v>
@@ -43201,7 +43201,7 @@
         </is>
       </c>
       <c r="B3290" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C3290" t="n">
         <v>0</v>
@@ -45983,7 +45983,7 @@
         </is>
       </c>
       <c r="B3504" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C3504" t="n">
         <v>0</v>
@@ -46074,7 +46074,7 @@
         </is>
       </c>
       <c r="B3511" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C3511" t="n">
         <v>0</v>
@@ -46243,7 +46243,7 @@
         </is>
       </c>
       <c r="B3524" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C3524" t="n">
         <v>0</v>
@@ -46451,7 +46451,7 @@
         </is>
       </c>
       <c r="B3540" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C3540" t="n">
         <v>0</v>
@@ -47803,7 +47803,7 @@
         </is>
       </c>
       <c r="B3644" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C3644" t="n">
         <v>0</v>
@@ -47842,7 +47842,7 @@
         </is>
       </c>
       <c r="B3647" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C3647" t="n">
         <v>0</v>
@@ -49285,7 +49285,7 @@
         </is>
       </c>
       <c r="B3758" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C3758" t="n">
         <v>0</v>
@@ -49337,7 +49337,7 @@
         </is>
       </c>
       <c r="B3762" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C3762" t="n">
         <v>1</v>
@@ -50845,7 +50845,7 @@
         </is>
       </c>
       <c r="B3878" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C3878" t="n">
         <v>0</v>
@@ -51014,7 +51014,7 @@
         </is>
       </c>
       <c r="B3891" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C3891" t="n">
         <v>0</v>
@@ -51625,7 +51625,7 @@
         </is>
       </c>
       <c r="B3938" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C3938" t="n">
         <v>0</v>
@@ -51664,7 +51664,7 @@
         </is>
       </c>
       <c r="B3941" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C3941" t="n">
         <v>0</v>
@@ -51898,7 +51898,7 @@
         </is>
       </c>
       <c r="B3959" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C3959" t="n">
         <v>0</v>
@@ -52392,7 +52392,7 @@
         </is>
       </c>
       <c r="B3997" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C3997" t="n">
         <v>0</v>
@@ -53029,7 +53029,7 @@
         </is>
       </c>
       <c r="B4046" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C4046" t="n">
         <v>0</v>
@@ -53055,7 +53055,7 @@
         </is>
       </c>
       <c r="B4048" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C4048" t="n">
         <v>0</v>
@@ -53705,7 +53705,7 @@
         </is>
       </c>
       <c r="B4098" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C4098" t="n">
         <v>0</v>
@@ -54537,7 +54537,7 @@
         </is>
       </c>
       <c r="B4162" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C4162" t="n">
         <v>0</v>
@@ -57579,7 +57579,7 @@
         </is>
       </c>
       <c r="B4396" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C4396" t="n">
         <v>1</v>
@@ -57605,7 +57605,7 @@
         </is>
       </c>
       <c r="B4398" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C4398" t="n">
         <v>0</v>
@@ -58203,7 +58203,7 @@
         </is>
       </c>
       <c r="B4444" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C4444" t="n">
         <v>0</v>
@@ -58294,7 +58294,7 @@
         </is>
       </c>
       <c r="B4451" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C4451" t="n">
         <v>0</v>
@@ -58853,7 +58853,7 @@
         </is>
       </c>
       <c r="B4494" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C4494" t="n">
         <v>0</v>
@@ -58879,7 +58879,7 @@
         </is>
       </c>
       <c r="B4496" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C4496" t="n">
         <v>0</v>
@@ -59386,7 +59386,7 @@
         </is>
       </c>
       <c r="B4535" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C4535" t="n">
         <v>0</v>
@@ -61869,7 +61869,7 @@
         </is>
       </c>
       <c r="B4726" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C4726" t="n">
         <v>0</v>
@@ -62896,7 +62896,7 @@
         </is>
       </c>
       <c r="B4805" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C4805" t="n">
         <v>0</v>
@@ -62948,7 +62948,7 @@
         </is>
       </c>
       <c r="B4809" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C4809" t="n">
         <v>0</v>
@@ -63052,7 +63052,7 @@
         </is>
       </c>
       <c r="B4817" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C4817" t="n">
         <v>0</v>
@@ -63117,7 +63117,7 @@
         </is>
       </c>
       <c r="B4822" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C4822" t="n">
         <v>0</v>
@@ -64040,7 +64040,7 @@
         </is>
       </c>
       <c r="B4893" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C4893" t="n">
         <v>0</v>
@@ -65327,7 +65327,7 @@
         </is>
       </c>
       <c r="B4992" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C4992" t="n">
         <v>1</v>
@@ -65821,7 +65821,7 @@
         </is>
       </c>
       <c r="B5030" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C5030" t="n">
         <v>1</v>
@@ -66432,7 +66432,7 @@
         </is>
       </c>
       <c r="B5077" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C5077" t="n">
         <v>0</v>
@@ -69110,7 +69110,7 @@
         </is>
       </c>
       <c r="B5283" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C5283" t="n">
         <v>0</v>
@@ -69643,7 +69643,7 @@
         </is>
       </c>
       <c r="B5324" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C5324" t="n">
         <v>0</v>
@@ -70280,7 +70280,7 @@
         </is>
       </c>
       <c r="B5373" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C5373" t="n">
         <v>0</v>
@@ -72776,7 +72776,7 @@
         </is>
       </c>
       <c r="B5565" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C5565" t="n">
         <v>0</v>
@@ -74115,7 +74115,7 @@
         </is>
       </c>
       <c r="B5668" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C5668" t="n">
         <v>0</v>
@@ -74557,7 +74557,7 @@
         </is>
       </c>
       <c r="B5702" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C5702" t="n">
         <v>1</v>
@@ -74778,7 +74778,7 @@
         </is>
       </c>
       <c r="B5719" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C5719" t="n">
         <v>0</v>
@@ -74882,7 +74882,7 @@
         </is>
       </c>
       <c r="B5727" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C5727" t="n">
         <v>0</v>
@@ -75415,7 +75415,7 @@
         </is>
       </c>
       <c r="B5768" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C5768" t="n">
         <v>0</v>
@@ -76221,7 +76221,7 @@
         </is>
       </c>
       <c r="B5830" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C5830" t="n">
         <v>0</v>
@@ -80030,7 +80030,7 @@
         </is>
       </c>
       <c r="B6123" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C6123" t="n">
         <v>0</v>
@@ -80095,7 +80095,7 @@
         </is>
       </c>
       <c r="B6128" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C6128" t="n">
         <v>0</v>
@@ -80147,7 +80147,7 @@
         </is>
       </c>
       <c r="B6132" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C6132" t="n">
         <v>0</v>

</xml_diff>